<commit_message>
chore: update database and gift list Excel files
Update the SQLite database and the gift list Excel file with the latest data.
</commit_message>
<xml_diff>
--- a/data/ListaPresentes.xlsx
+++ b/data/ListaPresentes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29725"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LucianoBastos\OneDrive\Projetos Pessoais\Casamento\PY_001 - Lista Presentes\7. Scripts\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/04bd3704f797149b/Projetos Pessoais/Casamento/PY_001 - Lista Presentes/7. Scripts/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF7D14EA-2731-4891-8764-321E050A1CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{CF7D14EA-2731-4891-8764-321E050A1CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85581E80-8686-42E0-AEEA-D0E27A94DE5B}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-1230" windowWidth="20730" windowHeight="11040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lista de Presentes" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="141">
   <si>
     <t>Presentes</t>
   </si>
@@ -445,6 +445,9 @@
   </si>
   <si>
     <t>https://shopee.com.br/product/521553964/18838172763?d_id=4c344&amp;uls_trackid=54rgsd7v00qf&amp;utm_content=4DMi5kAnNfJiG5ZJRdUtRohsWSUw</t>
+  </si>
+  <si>
+    <t>Azul</t>
   </si>
 </sst>
 </file>
@@ -711,8 +714,8 @@
   </sheetPr>
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1256,6 +1259,9 @@
       <c r="B58" s="3" t="s">
         <v>133</v>
       </c>
+      <c r="D58" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
@@ -1271,6 +1277,9 @@
       </c>
       <c r="B60" s="3" t="s">
         <v>137</v>
+      </c>
+      <c r="D60" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>